<commit_message>
Added ability to load excel 2007 file.
</commit_message>
<xml_diff>
--- a/gui/src/test/resources/catalogue.xlsx
+++ b/gui/src/test/resources/catalogue.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="8760"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="23420" windowHeight="12520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Special Shoe</t>
   </si>
   <si>
     <t>Special Toaster</t>
+  </si>
+  <si>
+    <t>2165165412655</t>
+  </si>
+  <si>
+    <t>4905524449563</t>
+  </si>
+  <si>
+    <t>51651651634</t>
   </si>
 </sst>
 </file>
@@ -57,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,33 +378,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>51651651634</v>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2165165412655</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4905524449563</v>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -397,6 +412,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -406,9 +426,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -418,8 +443,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>